<commit_message>
time and date added
</commit_message>
<xml_diff>
--- a/ex31/my_file.xlsx
+++ b/ex31/my_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/abf6ef98c0652b38/Área de Trabalho/PhytonCodes/ex31/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_1B25513CD626C3050616B72F0F9EE70A757B9A50" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4256F73-F0D3-473D-AA36-B26673E4FE7D}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_6CF529E2161A9D940D4E536AEFABCA8970706EFC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A7F899A-7363-4F69-84BB-6768BB6F9239}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,13 +372,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>